<commit_message>
units out of non-micro lab test
</commit_message>
<xml_diff>
--- a/Load/ontology/label_templates/lab_test_template_non-microbiology.xlsx
+++ b/Load/ontology/label_templates/lab_test_template_non-microbiology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/label_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B71637-C920-284F-9A42-36275A6354CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8887569F-D283-6D40-A4A0-70108F518B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_detection_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>variable</t>
   </si>
@@ -130,6 +134,9 @@
   </si>
   <si>
     <t>TNFA concentration</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
 </sst>
 </file>
@@ -974,13 +981,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3:H19"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,7 +1003,7 @@
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,8 +1031,11 @@
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="125" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1056,15 +1066,19 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f>TRIM(UPPER(LEFT(C3,1))&amp;RIGHT(C3,LEN(C3)-1)&amp;IF(D3="",""," ("&amp;D3&amp;")")&amp;IF(E3="","",", "&amp;E3)&amp;IF(F3="","",", at "&amp;F3))</f>
-        <v>IL-1b concentration (pg/mL)</v>
+        <f>TRIM(UPPER(LEFT(C3,1))&amp;RIGHT(C3,LEN(C3)-1)&amp;IF(E3="","",", "&amp;E3)&amp;IF(F3="","",", at "&amp;F3))</f>
+        <v>IL-1b concentration</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I32" si="0">TRIM(UPPER(LEFT(B3,1))&amp;RIGHT(B3,LEN(B3)-1)&amp;" test")</f>
-        <v>Maternal breast milk test</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I3:I19" si="0">TRIM(UPPER(LEFT(B3,1))&amp;RIGHT(B3,LEN(B3)-1)&amp;" test")</f>
+        <v>Maternal breast milk test</v>
+      </c>
+      <c r="J3" s="1" t="str">
+        <f>IF(D3="","",D3)</f>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1075,15 +1089,19 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f t="shared" ref="H4:H32" si="1">TRIM(UPPER(LEFT(C4,1))&amp;RIGHT(C4,LEN(C4)-1)&amp;IF(D4="",""," ("&amp;D4&amp;")")&amp;IF(E4="","",", "&amp;E4)&amp;IF(F4="","",", at "&amp;F4))</f>
-        <v>IL-2 concentration (pg/mL)</v>
+        <f t="shared" ref="H4:H19" si="1">TRIM(UPPER(LEFT(C4,1))&amp;RIGHT(C4,LEN(C4)-1)&amp;IF(E4="","",", "&amp;E4)&amp;IF(F4="","",", at "&amp;F4))</f>
+        <v>IL-2 concentration</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J4" s="1" t="str">
+        <f t="shared" ref="J4:J19" si="2">IF(D4="","",D4)</f>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1095,14 +1113,18 @@
       </c>
       <c r="H5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-4 concentration (pg/mL)</v>
+        <v>IL-4 concentration</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1114,14 +1136,18 @@
       </c>
       <c r="H6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-5 concentration (pg/mL)</v>
+        <v>IL-5 concentration</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1133,14 +1159,18 @@
       </c>
       <c r="H7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-6 concentration (pg/mL)</v>
+        <v>IL-6 concentration</v>
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1152,14 +1182,18 @@
       </c>
       <c r="H8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-7 concentration (pg/mL)</v>
+        <v>IL-7 concentration</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1171,14 +1205,18 @@
       </c>
       <c r="H9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-8 concentration (pg/mL)</v>
+        <v>IL-8 concentration</v>
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1190,14 +1228,18 @@
       </c>
       <c r="H10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-10 concentration (pg/mL)</v>
+        <v>IL-10 concentration</v>
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1209,14 +1251,18 @@
       </c>
       <c r="H11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-12p70 concentration (pg/mL)</v>
+        <v>IL-12p70 concentration</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1228,14 +1274,18 @@
       </c>
       <c r="H12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-13 concentration (pg/mL)</v>
+        <v>IL-13 concentration</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1247,14 +1297,18 @@
       </c>
       <c r="H13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IL-17A concentration (pg/mL)</v>
+        <v>IL-17A concentration</v>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1266,14 +1320,18 @@
       </c>
       <c r="H14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>G-CSF concentration (pg/mL)</v>
+        <v>G-CSF concentration</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1285,14 +1343,18 @@
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>GM-CSF concentration (pg/mL)</v>
+        <v>GM-CSF concentration</v>
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1304,14 +1366,18 @@
       </c>
       <c r="H16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IFNG concentration (pg/mL)</v>
+        <v>IFNG concentration</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1323,14 +1389,18 @@
       </c>
       <c r="H17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MCP-1(MCAF) concentration (pg/mL)</v>
+        <v>MCP-1(MCAF) concentration</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1342,14 +1412,18 @@
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MIP1b concentration (pg/mL)</v>
+        <v>MIP1b concentration</v>
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1361,50 +1435,54 @@
       </c>
       <c r="H19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TNFA concentration (pg/mL)</v>
+        <v>TNFA concentration</v>
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Maternal breast milk test</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>pg/mL</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C20"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C21"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C22"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C23"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C24"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C25"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C26"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C27"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C28"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C29"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C30"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C31"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C32"/>
     </row>
   </sheetData>

</xml_diff>